<commit_message>
all the team names
</commit_message>
<xml_diff>
--- a/static/Team Registration.xlsx
+++ b/static/Team Registration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1360" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="-200" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="309">
   <si>
     <t>Team Name</t>
   </si>
@@ -158,9 +158,6 @@
     <t>akeenjames@gmail.com</t>
   </si>
   <si>
-    <t>FAMP</t>
-  </si>
-  <si>
     <t>Peter Yin</t>
   </si>
   <si>
@@ -279,13 +276,688 @@
   </si>
   <si>
     <t>nwk.lee.a@hotmail.com</t>
+  </si>
+  <si>
+    <t>The Wolves of IV</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Mikaela Guerrero</t>
+  </si>
+  <si>
+    <t>mikaelaguerrero@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Angel Chavez</t>
+  </si>
+  <si>
+    <t>angelchavez@ucsb.edu</t>
+  </si>
+  <si>
+    <t>CarrotCake</t>
+  </si>
+  <si>
+    <t>Sergio Zambrano</t>
+  </si>
+  <si>
+    <t>zambranoguerra@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Rebecca He</t>
+  </si>
+  <si>
+    <t>zhiqinghe@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Rosé</t>
+  </si>
+  <si>
+    <t>Ziwei Zhang</t>
+  </si>
+  <si>
+    <t>ziweizhang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Univa Song</t>
+  </si>
+  <si>
+    <t>x_song@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Yuhan Ling</t>
+  </si>
+  <si>
+    <t>7th floor</t>
+  </si>
+  <si>
+    <t>Kennard Peters</t>
+  </si>
+  <si>
+    <t>kennardpeters@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jason Gonzalez</t>
+  </si>
+  <si>
+    <t>jasongonzalez@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Angel Hernandez</t>
+  </si>
+  <si>
+    <t>angel_hernandez@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Limp Eggnog</t>
+  </si>
+  <si>
+    <t>Adam Mendenhall</t>
+  </si>
+  <si>
+    <t>amendenhall@ucsb.edu</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foad Nabi Bidhendi </t>
+  </si>
+  <si>
+    <t>foad@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Shkreli Bros</t>
+  </si>
+  <si>
+    <t>Joel Holsinger</t>
+  </si>
+  <si>
+    <t>joelholsinger@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Lawrencedlin@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Lawrence Lin</t>
+  </si>
+  <si>
+    <t>Team Avatar</t>
+  </si>
+  <si>
+    <t>Grant Nolasco</t>
+  </si>
+  <si>
+    <t>gnolasco@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Candace McKeag</t>
+  </si>
+  <si>
+    <t>cjmckeag@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Aaron Barel</t>
+  </si>
+  <si>
+    <t>aaron_barel@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Eri Kawakami</t>
+  </si>
+  <si>
+    <t>ekawakami@ucsb.edu</t>
+  </si>
+  <si>
+    <t>VB&amp;F</t>
+  </si>
+  <si>
+    <t>Elia(Yiyi) Xu</t>
+  </si>
+  <si>
+    <t>yiyi_xu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Yiwei Li</t>
+  </si>
+  <si>
+    <t>yiweili@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Anqi Jiang</t>
+  </si>
+  <si>
+    <t>anqijiang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Little White</t>
+  </si>
+  <si>
+    <t>Jinglin Liu</t>
+  </si>
+  <si>
+    <t>jinglinliu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Weiqing Qi</t>
+  </si>
+  <si>
+    <t>weiqing@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Xinyu He</t>
+  </si>
+  <si>
+    <t>xinyuhe@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Kaiyi Yang</t>
+  </si>
+  <si>
+    <t>kaiyi@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jeffery Cole</t>
+  </si>
+  <si>
+    <t>jcole@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Subprime Quality</t>
+  </si>
+  <si>
+    <t>David Joe</t>
+  </si>
+  <si>
+    <t>davidejoe@ucsb.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dennis Wang </t>
+  </si>
+  <si>
+    <t>Renwang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Megan Handa</t>
+  </si>
+  <si>
+    <t>mhanda@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Dorothy Li</t>
+  </si>
+  <si>
+    <t>dorothyli@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Chow RunFast</t>
+  </si>
+  <si>
+    <t>Syen Yang Lu</t>
+  </si>
+  <si>
+    <t>syenyang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jiaxi Ye</t>
+  </si>
+  <si>
+    <t>jiaxi@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Ke Wang</t>
+  </si>
+  <si>
+    <t>wang11@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Yue Fei</t>
+  </si>
+  <si>
+    <t>fei@ucsb.edu</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>Meet Gala</t>
+  </si>
+  <si>
+    <t>meet@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jack Pham</t>
+  </si>
+  <si>
+    <t>l_pham00@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Chuqiao Liu</t>
+  </si>
+  <si>
+    <t>chuqiao@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Adam Ritcher</t>
+  </si>
+  <si>
+    <t>adamritcher@gmail.com</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Ethan Scott</t>
+  </si>
+  <si>
+    <t>ethanscott@ucsb.edu</t>
+  </si>
+  <si>
+    <t>James W Squad</t>
+  </si>
+  <si>
+    <t>James Wakabayashi</t>
+  </si>
+  <si>
+    <t>jwakabayashi@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Riley's Team</t>
+  </si>
+  <si>
+    <t>Riley Mault</t>
+  </si>
+  <si>
+    <t>rmault@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Team Accuracy</t>
+  </si>
+  <si>
+    <t>Lily Li</t>
+  </si>
+  <si>
+    <t>ziwan_li@ucsb.edu</t>
+  </si>
+  <si>
+    <t>kejialiu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Alice Liu</t>
+  </si>
+  <si>
+    <t>Jack Pan</t>
+  </si>
+  <si>
+    <t>hpan@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jiayi Chen</t>
+  </si>
+  <si>
+    <t>jiayichen@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Tamias</t>
+  </si>
+  <si>
+    <t>Tim Jou</t>
+  </si>
+  <si>
+    <t>Timothyejou@gmail.com</t>
+  </si>
+  <si>
+    <t>Rita Mounir</t>
+  </si>
+  <si>
+    <t>ritamounir@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Mana Sanavi</t>
+  </si>
+  <si>
+    <t>msanavi.ms@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulnoza Bobokalonova </t>
+  </si>
+  <si>
+    <t>gulnoz.bobok@gmail.com</t>
+  </si>
+  <si>
+    <t>walnuts</t>
+  </si>
+  <si>
+    <t>Bryan Xu</t>
+  </si>
+  <si>
+    <t>bryanxu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Justin Wang</t>
+  </si>
+  <si>
+    <t>jwang616@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Emily Lou</t>
+  </si>
+  <si>
+    <t>emilytlou@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Daniel Guo</t>
+  </si>
+  <si>
+    <t>dguo@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Sharpe Predictions</t>
+  </si>
+  <si>
+    <t>Sam O'Neill</t>
+  </si>
+  <si>
+    <t>sroneill@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Axolotls</t>
+  </si>
+  <si>
+    <t>Geneva Schlafly</t>
+  </si>
+  <si>
+    <t>gschlafly@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Sean Costello</t>
+  </si>
+  <si>
+    <t>seancostello@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jason Gros</t>
+  </si>
+  <si>
+    <t>jgros@ucsb.edu</t>
+  </si>
+  <si>
+    <t>HKHK</t>
+  </si>
+  <si>
+    <t>Connor Keller</t>
+  </si>
+  <si>
+    <t>connorkeller@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Peter Harano</t>
+  </si>
+  <si>
+    <t>peterharano@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jake Hieber</t>
+  </si>
+  <si>
+    <t>Jakehieber@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Nino Kim</t>
+  </si>
+  <si>
+    <t>ninokim@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Just For Fun</t>
+  </si>
+  <si>
+    <t>Yuxiao Luo</t>
+  </si>
+  <si>
+    <t>yuxiaoluo@ucsb.edu</t>
+  </si>
+  <si>
+    <t>*Same team name as first team</t>
+  </si>
+  <si>
+    <t>Army of One</t>
+  </si>
+  <si>
+    <t>Anthony Castillo</t>
+  </si>
+  <si>
+    <t>acastillo@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Lehman’s Last Analysts</t>
+  </si>
+  <si>
+    <t>Andrew Morissette</t>
+  </si>
+  <si>
+    <t>amorissette@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Aram Dovlatyan</t>
+  </si>
+  <si>
+    <t>aramdovlatyan@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Marty Chen</t>
+  </si>
+  <si>
+    <t>Hchen@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Sahaj Makharia</t>
+  </si>
+  <si>
+    <t>Sahaj@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Model Behavior</t>
+  </si>
+  <si>
+    <t>Shaiyon Hariri</t>
+  </si>
+  <si>
+    <t>shaiyon@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Muhtadi Mahmud</t>
+  </si>
+  <si>
+    <t>muhtadi@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Yash Rane</t>
+  </si>
+  <si>
+    <t>yash_rane@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Amanda Ho</t>
+  </si>
+  <si>
+    <t>Amandaho@ucsb.edu</t>
+  </si>
+  <si>
+    <t>TBADAAAR</t>
+  </si>
+  <si>
+    <t>Spencer Andrews</t>
+  </si>
+  <si>
+    <t>spencer_andrews@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>Victor Huang</t>
+  </si>
+  <si>
+    <t>chuanhanhuang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Sophia Song</t>
+  </si>
+  <si>
+    <t>shuyao@ucsb.edu</t>
+  </si>
+  <si>
+    <t>The World History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shinnosuke Kaneko </t>
+  </si>
+  <si>
+    <t>shinnosuke_kaneko@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Thien An Nguyen</t>
+  </si>
+  <si>
+    <t>tanguyen@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Zenith</t>
+  </si>
+  <si>
+    <t>Zijie Fang</t>
+  </si>
+  <si>
+    <t>zijie_fang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Ester Hsu</t>
+  </si>
+  <si>
+    <t>eahsu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Hongshan Lin</t>
+  </si>
+  <si>
+    <t>h_lin@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Manpal Sidhu</t>
+  </si>
+  <si>
+    <t>manpalssidhu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Jungle</t>
+  </si>
+  <si>
+    <t>Xing Su</t>
+  </si>
+  <si>
+    <t>xingsu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Ximei Wu</t>
+  </si>
+  <si>
+    <t>ximei_wu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Chi Xu</t>
+  </si>
+  <si>
+    <t>chi_xu@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Changhao Li</t>
+  </si>
+  <si>
+    <t>changhaoli@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Cheesecake</t>
+  </si>
+  <si>
+    <t>RUOYANG FENG</t>
+  </si>
+  <si>
+    <t>ruoyang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>YUXIN YANG</t>
+  </si>
+  <si>
+    <t>yuxinyang@ucsb.edu</t>
+  </si>
+  <si>
+    <t>WENJIAN LI</t>
+  </si>
+  <si>
+    <t>wenjianli@ucsb.edu</t>
+  </si>
+  <si>
+    <t>The Partial Derivatives</t>
+  </si>
+  <si>
+    <t>Drew Pritchard</t>
+  </si>
+  <si>
+    <t>drewpritchard@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Candace Mckeag</t>
+  </si>
+  <si>
+    <t>Coop</t>
+  </si>
+  <si>
+    <t>Evan Azevedo</t>
+  </si>
+  <si>
+    <t>eazevedo@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Big Brother</t>
+  </si>
+  <si>
+    <t>Shaocong Ma</t>
+  </si>
+  <si>
+    <t>shaocongma@ucsb.edu</t>
+  </si>
+  <si>
+    <t>Chi-Square</t>
+  </si>
+  <si>
+    <t>Yihao Gao</t>
+  </si>
+  <si>
+    <t>yihao@ucsb.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuxin Zhang </t>
+  </si>
+  <si>
+    <t>yuxin_zhang@ucsb.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xinxin Lin </t>
+  </si>
+  <si>
+    <t>xinxinlin@ucsb.edu</t>
+  </si>
+  <si>
+    <t>MSSerp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -300,6 +972,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -329,11 +1006,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -612,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,162 +1485,1055 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
         <v>68</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" t="s">
         <v>80</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>84</v>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+      <c r="B57" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B59" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B60" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B61" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+      <c r="B64" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="2"/>
+      <c r="B65" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B67" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B68" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B69" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="2"/>
+      <c r="B71" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="2"/>
+      <c r="B72" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="2"/>
+      <c r="B73" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C74" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>179</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="2"/>
+      <c r="B78" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="2"/>
+      <c r="B79" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="2"/>
+      <c r="B80" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>191</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C81" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B82" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C82" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B83" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B84" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C84" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="2"/>
+      <c r="B86" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>209</v>
+      </c>
+      <c r="B89" t="s">
+        <v>210</v>
+      </c>
+      <c r="C89" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>219</v>
+      </c>
+      <c r="B93" t="s">
+        <v>220</v>
+      </c>
+      <c r="C93" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>224</v>
+      </c>
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>232</v>
+      </c>
+      <c r="B98" t="s">
+        <v>233</v>
+      </c>
+      <c r="C98" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>244</v>
+      </c>
+      <c r="B103" t="s">
+        <v>245</v>
+      </c>
+      <c r="C103" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>247</v>
+      </c>
+      <c r="C104" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>249</v>
+      </c>
+      <c r="C105" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>251</v>
+      </c>
+      <c r="C106" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>256</v>
+      </c>
+      <c r="B108" t="s">
+        <v>257</v>
+      </c>
+      <c r="C108" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>259</v>
+      </c>
+      <c r="C109" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>266</v>
+      </c>
+      <c r="B112" t="s">
+        <v>267</v>
+      </c>
+      <c r="C112" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>269</v>
+      </c>
+      <c r="C113" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>271</v>
+      </c>
+      <c r="C114" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>275</v>
+      </c>
+      <c r="B116" t="s">
+        <v>276</v>
+      </c>
+      <c r="C116" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>278</v>
+      </c>
+      <c r="C117" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>280</v>
+      </c>
+      <c r="C118" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>282</v>
+      </c>
+      <c r="C119" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="2"/>
+      <c r="B122" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>291</v>
+      </c>
+      <c r="B123" t="s">
+        <v>292</v>
+      </c>
+      <c r="C123" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
+        <v>294</v>
+      </c>
+      <c r="C124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>298</v>
+      </c>
+      <c r="B126" t="s">
+        <v>299</v>
+      </c>
+      <c r="C126" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -995,6 +2572,8 @@
     <hyperlink ref="C33" r:id="rId32"/>
     <hyperlink ref="C34" r:id="rId33"/>
     <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C37" r:id="rId35"/>
+    <hyperlink ref="C54" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>